<commit_message>
popup for exports excel
</commit_message>
<xml_diff>
--- a/ouputFiles/excel-from-js.xlsx
+++ b/ouputFiles/excel-from-js.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -399,126 +399,24 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="B2" t="str">
-        <v>7</v>
+        <v>112</v>
       </c>
       <c r="C2" t="str">
-        <v>Maria Zulin.</v>
+        <v>Marciana Garay.</v>
       </c>
       <c r="D2" t="str">
         <v>si</v>
       </c>
       <c r="E2" t="str">
-        <v>Ganador de Gs. 1.000.000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3">
-        <v>11</v>
-      </c>
-      <c r="B3" t="str">
-        <v>11</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Silvia Fariña.</v>
-      </c>
-      <c r="D3" t="str">
-        <v>si</v>
-      </c>
-      <c r="E3" t="str">
-        <v>Ganador de Gs. 1.000.000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4">
-        <v>22</v>
-      </c>
-      <c r="B4" t="str">
-        <v>22</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Silvia Diaz.</v>
-      </c>
-      <c r="D4" t="str">
-        <v>si</v>
-      </c>
-      <c r="E4" t="str">
-        <v>Ganador de Gs. 1.000.000</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5">
-        <v>39</v>
-      </c>
-      <c r="B5" t="str">
-        <v>39</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Rhutt Gaona.</v>
-      </c>
-      <c r="D5" t="str">
-        <v>si</v>
-      </c>
-      <c r="E5" t="str">
-        <v>Ganador de Gs. 1.000.000</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6">
-        <v>100</v>
-      </c>
-      <c r="B6" t="str">
-        <v>100</v>
-      </c>
-      <c r="C6" t="str">
-        <v xml:space="preserve">Sonia Quiroga De Alvarenga. </v>
-      </c>
-      <c r="D6" t="str">
-        <v>si</v>
-      </c>
-      <c r="E6" t="str">
-        <v>Ganador de Gs. 1.000.000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7">
-        <v>104</v>
-      </c>
-      <c r="B7" t="str">
-        <v>104</v>
-      </c>
-      <c r="C7" t="str">
-        <v>Samantha Alvarenga.</v>
-      </c>
-      <c r="D7" t="str">
-        <v>si</v>
-      </c>
-      <c r="E7" t="str">
-        <v>Ganador de Gs. 1.000.000</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8">
-        <v>108</v>
-      </c>
-      <c r="B8" t="str">
-        <v>108</v>
-      </c>
-      <c r="C8" t="str">
-        <v>Lourdes Zelada.</v>
-      </c>
-      <c r="D8" t="str">
-        <v>si</v>
-      </c>
-      <c r="E8" t="str">
         <v>Ganador de Gs. 1.000.000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
first commit to deploy branch
</commit_message>
<xml_diff>
--- a/ouputFiles/excel-from-js.xlsx
+++ b/ouputFiles/excel-from-js.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -388,7 +388,7 @@
         <v>Socio numero</v>
       </c>
       <c r="C1" t="str">
-        <v>Nmbre y Apellido</v>
+        <v>Nombre y Apellido</v>
       </c>
       <c r="D1" t="str">
         <v>Ganador</v>
@@ -399,24 +399,58 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="B2" t="str">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="C2" t="str">
-        <v>Marciana Garay.</v>
+        <v>Sergio Riquelme.</v>
       </c>
       <c r="D2" t="str">
         <v>si</v>
       </c>
       <c r="E2" t="str">
+        <v>Ganador de Gs. 1.000.000</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>18</v>
+      </c>
+      <c r="B3" t="str">
+        <v>18</v>
+      </c>
+      <c r="C3" t="str">
+        <v>Jorge Morinigo.</v>
+      </c>
+      <c r="D3" t="str">
+        <v>si</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Ganador de Gs. 1.000.000</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>74</v>
+      </c>
+      <c r="B4" t="str">
+        <v>74</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Stella Martinez.</v>
+      </c>
+      <c r="D4" t="str">
+        <v>si</v>
+      </c>
+      <c r="E4" t="str">
         <v>Ganador de Gs. 1.000.000</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>